<commit_message>
I don't know why I keep doing any of this.
</commit_message>
<xml_diff>
--- a/data-raw/turnips/turnips.xlsx
+++ b/data-raw/turnips/turnips.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="6">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -113,7 +113,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -123,6 +123,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,13 +147,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1289"/>
+  <dimension ref="A1:C1382"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1252" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1290" activeCellId="0" sqref="A1290"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1299" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1321" activeCellId="0" sqref="A1321"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="17.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -14310,6 +14314,1029 @@
       </c>
       <c r="C1289" s="0" t="n">
         <v>93</v>
+      </c>
+    </row>
+    <row r="1290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1290" s="2" t="n">
+        <v>44991</v>
+      </c>
+      <c r="B1290" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1290" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="1291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1291" s="2" t="n">
+        <v>44992</v>
+      </c>
+      <c r="B1291" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1291" s="0" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="1292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1292" s="2" t="n">
+        <v>44992</v>
+      </c>
+      <c r="B1292" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1292" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1293" s="2" t="n">
+        <v>44993</v>
+      </c>
+      <c r="B1293" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1293" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1294" s="2" t="n">
+        <v>44993</v>
+      </c>
+      <c r="B1294" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1294" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="1295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1295" s="2" t="n">
+        <v>44994</v>
+      </c>
+      <c r="B1295" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1295" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1296" s="2" t="n">
+        <v>44994</v>
+      </c>
+      <c r="B1296" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1296" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1297" s="2" t="n">
+        <v>44995</v>
+      </c>
+      <c r="B1297" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1297" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="1298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1298" s="2" t="n">
+        <v>44995</v>
+      </c>
+      <c r="B1298" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1298" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1299" s="2" t="n">
+        <v>44996</v>
+      </c>
+      <c r="B1299" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1299" s="0" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1300" s="2" t="n">
+        <v>44996</v>
+      </c>
+      <c r="B1300" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1300" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1301" s="2" t="n">
+        <v>44997</v>
+      </c>
+      <c r="B1301" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1301" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="1302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1302" s="2" t="n">
+        <v>44998</v>
+      </c>
+      <c r="B1302" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1302" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="1303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1303" s="2" t="n">
+        <v>44998</v>
+      </c>
+      <c r="B1303" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1303" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1304" s="2" t="n">
+        <v>44999</v>
+      </c>
+      <c r="B1304" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1304" s="0" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1305" s="2" t="n">
+        <v>44999</v>
+      </c>
+      <c r="B1305" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1305" s="0" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1306" s="2" t="n">
+        <v>45000</v>
+      </c>
+      <c r="B1306" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1306" s="0" t="n">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="1307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1307" s="2" t="n">
+        <v>45000</v>
+      </c>
+      <c r="B1307" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1307" s="0" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1308" s="2" t="n">
+        <v>45001</v>
+      </c>
+      <c r="B1308" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1308" s="0" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1309" s="2" t="n">
+        <v>45001</v>
+      </c>
+      <c r="B1309" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1309" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1310" s="2" t="n">
+        <v>45002</v>
+      </c>
+      <c r="B1310" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1310" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1311" s="2" t="n">
+        <v>45002</v>
+      </c>
+      <c r="B1311" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1311" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="1312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1312" s="2" t="n">
+        <v>45003</v>
+      </c>
+      <c r="B1312" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1312" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1313" s="2" t="n">
+        <v>45003</v>
+      </c>
+      <c r="B1313" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1313" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1314" s="2" t="n">
+        <v>45004</v>
+      </c>
+      <c r="B1314" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1314" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1315" s="2" t="n">
+        <v>45005</v>
+      </c>
+      <c r="B1315" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1315" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="1316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1316" s="2" t="n">
+        <v>45005</v>
+      </c>
+      <c r="B1316" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1316" s="0" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="1317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1317" s="2" t="n">
+        <v>45006</v>
+      </c>
+      <c r="B1317" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1317" s="0" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="1318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1318" s="2" t="n">
+        <v>45006</v>
+      </c>
+      <c r="B1318" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1318" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1319" s="2" t="n">
+        <v>45007</v>
+      </c>
+      <c r="B1319" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1319" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1320" s="2" t="n">
+        <v>45007</v>
+      </c>
+      <c r="B1320" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1320" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1321" s="2" t="n">
+        <v>45008</v>
+      </c>
+      <c r="B1321" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1321" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1322" s="2" t="n">
+        <v>45008</v>
+      </c>
+      <c r="B1322" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1322" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="1323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1323" s="2" t="n">
+        <v>45009</v>
+      </c>
+      <c r="B1323" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1323" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1324" s="2" t="n">
+        <v>45009</v>
+      </c>
+      <c r="B1324" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1324" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1325" s="2" t="n">
+        <v>45010</v>
+      </c>
+      <c r="B1325" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1325" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1326" s="2" t="n">
+        <v>45010</v>
+      </c>
+      <c r="B1326" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1326" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1327" s="2" t="n">
+        <v>45011</v>
+      </c>
+      <c r="B1327" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1327" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="1328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1328" s="2" t="n">
+        <v>45012</v>
+      </c>
+      <c r="B1328" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1328" s="0" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1329" s="2" t="n">
+        <v>45012</v>
+      </c>
+      <c r="B1329" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1329" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1330" s="2" t="n">
+        <v>45013</v>
+      </c>
+      <c r="B1330" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1330" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="1331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1331" s="2" t="n">
+        <v>45013</v>
+      </c>
+      <c r="B1331" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1331" s="0" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="1332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1332" s="2" t="n">
+        <v>45014</v>
+      </c>
+      <c r="B1332" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1332" s="0" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1333" s="2" t="n">
+        <v>45014</v>
+      </c>
+      <c r="B1333" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1333" s="0" t="n">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="1334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1334" s="2" t="n">
+        <v>45015</v>
+      </c>
+      <c r="B1334" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1334" s="0" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1335" s="2" t="n">
+        <v>45015</v>
+      </c>
+      <c r="B1335" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1335" s="0" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="1336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1336" s="2" t="n">
+        <v>45016</v>
+      </c>
+      <c r="B1336" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1336" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1337" s="2" t="n">
+        <v>45016</v>
+      </c>
+      <c r="B1337" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1337" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1338" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B1338" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1338" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1339" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B1339" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1339" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1340" s="2" t="n">
+        <v>45018</v>
+      </c>
+      <c r="B1340" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1340" s="0" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="1341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1341" s="2" t="n">
+        <v>45019</v>
+      </c>
+      <c r="B1341" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1341" s="0" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="1342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1342" s="2" t="n">
+        <v>45019</v>
+      </c>
+      <c r="B1342" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1342" s="0" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="1343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1343" s="2" t="n">
+        <v>45020</v>
+      </c>
+      <c r="B1343" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1343" s="0" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="1344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1344" s="2" t="n">
+        <v>45020</v>
+      </c>
+      <c r="B1344" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1344" s="0" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="1345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1345" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="B1345" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1345" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1346" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="B1346" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1346" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1347" s="2" t="n">
+        <v>45022</v>
+      </c>
+      <c r="B1347" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1347" s="0" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1348" s="2" t="n">
+        <v>45022</v>
+      </c>
+      <c r="B1348" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1348" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="1349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1349" s="2" t="n">
+        <v>45023</v>
+      </c>
+      <c r="B1349" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1349" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1350" s="2" t="n">
+        <v>45023</v>
+      </c>
+      <c r="B1350" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1350" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1351" s="2" t="n">
+        <v>45024</v>
+      </c>
+      <c r="B1351" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1351" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1352" s="2" t="n">
+        <v>45024</v>
+      </c>
+      <c r="B1352" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1352" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1353" s="2" t="n">
+        <v>45025</v>
+      </c>
+      <c r="B1353" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1353" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1354" s="2" t="n">
+        <v>45026</v>
+      </c>
+      <c r="B1354" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1354" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="1355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1355" s="2" t="n">
+        <v>45026</v>
+      </c>
+      <c r="B1355" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1355" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="1356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1356" s="2" t="n">
+        <v>45027</v>
+      </c>
+      <c r="B1356" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1356" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1357" s="2" t="n">
+        <v>45027</v>
+      </c>
+      <c r="B1357" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1357" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1358" s="2" t="n">
+        <v>45028</v>
+      </c>
+      <c r="B1358" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1358" s="0" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1359" s="2" t="n">
+        <v>45028</v>
+      </c>
+      <c r="B1359" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1359" s="0" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1360" s="2" t="n">
+        <v>45029</v>
+      </c>
+      <c r="B1360" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1360" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="1361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1361" s="2" t="n">
+        <v>45029</v>
+      </c>
+      <c r="B1361" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1361" s="0" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1362" s="2" t="n">
+        <v>45030</v>
+      </c>
+      <c r="B1362" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1362" s="0" t="n">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="1363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1363" s="2" t="n">
+        <v>45030</v>
+      </c>
+      <c r="B1363" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1363" s="0" t="n">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="1364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1364" s="2" t="n">
+        <v>45031</v>
+      </c>
+      <c r="B1364" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1364" s="0" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="1365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1365" s="2" t="n">
+        <v>45031</v>
+      </c>
+      <c r="B1365" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1365" s="0" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="1366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1366" s="2" t="n">
+        <v>45032</v>
+      </c>
+      <c r="B1366" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1366" s="0" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1367" s="2" t="n">
+        <v>45033</v>
+      </c>
+      <c r="B1367" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1367" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1368" s="2" t="n">
+        <v>45033</v>
+      </c>
+      <c r="B1368" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1368" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="1369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1369" s="2" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B1369" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1369" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="1370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1370" s="2" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B1370" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1370" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1371" s="2" t="n">
+        <v>45035</v>
+      </c>
+      <c r="B1371" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1371" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1372" s="2" t="n">
+        <v>45035</v>
+      </c>
+      <c r="B1372" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1372" s="0" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1373" s="2" t="n">
+        <v>45036</v>
+      </c>
+      <c r="B1373" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1373" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="1374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1374" s="2" t="n">
+        <v>45036</v>
+      </c>
+      <c r="B1374" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1374" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1375" s="2" t="n">
+        <v>45037</v>
+      </c>
+      <c r="B1375" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1375" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="1376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1376" s="2" t="n">
+        <v>45037</v>
+      </c>
+      <c r="B1376" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1376" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1377" s="2" t="n">
+        <v>45038</v>
+      </c>
+      <c r="B1377" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1377" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1378" s="2" t="n">
+        <v>45038</v>
+      </c>
+      <c r="B1378" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1378" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1379" s="2" t="n">
+        <v>45039</v>
+      </c>
+      <c r="B1379" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1379" s="0" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1380" s="2" t="n">
+        <v>45040</v>
+      </c>
+      <c r="B1380" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1380" s="0" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="1381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1381" s="3" t="n">
+        <v>45040</v>
+      </c>
+      <c r="B1381" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1381" s="0" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1382" s="2" t="n">
+        <v>45041</v>
+      </c>
+      <c r="B1382" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1382" s="0" t="n">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
end of the turnips
</commit_message>
<xml_diff>
--- a/data-raw/turnips/turnips.xlsx
+++ b/data-raw/turnips/turnips.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="6">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -147,13 +147,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1419"/>
+  <dimension ref="A1:C1430"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1382" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1420" activeCellId="0" sqref="A1420"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1394" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1431" activeCellId="0" sqref="A1431"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.1015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -15744,6 +15744,127 @@
       </c>
       <c r="C1419" s="0" t="n">
         <v>75</v>
+      </c>
+    </row>
+    <row r="1420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1420" s="2" t="n">
+        <v>45061</v>
+      </c>
+      <c r="B1420" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1420" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1421" s="2" t="n">
+        <v>45062</v>
+      </c>
+      <c r="B1421" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1421" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1422" s="2" t="n">
+        <v>45062</v>
+      </c>
+      <c r="B1422" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1422" s="0" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1423" s="2" t="n">
+        <v>45063</v>
+      </c>
+      <c r="B1423" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1423" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1424" s="2" t="n">
+        <v>45063</v>
+      </c>
+      <c r="B1424" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1424" s="0" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1425" s="2" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B1425" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1425" s="0" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1426" s="2" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B1426" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1426" s="0" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1427" s="2" t="n">
+        <v>45065</v>
+      </c>
+      <c r="B1427" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1427" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="1428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1428" s="2" t="n">
+        <v>45065</v>
+      </c>
+      <c r="B1428" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1428" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1429" s="2" t="n">
+        <v>45066</v>
+      </c>
+      <c r="B1429" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1429" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="1430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1430" s="2" t="n">
+        <v>45066</v>
+      </c>
+      <c r="B1430" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1430" s="0" t="n">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>